<commit_message>
Dodanie podsumowanie i raportu z testów
</commit_message>
<xml_diff>
--- a/dokumentacja/Karta testów - Dariusz Waltoś.xlsx
+++ b/dokumentacja/Karta testów - Dariusz Waltoś.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
   <si>
     <t>Nazwisko</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Obsługa kalendarza</t>
+  </si>
+  <si>
+    <t>Brak walidacji czy wprowadzona liczba jest stringiem</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -532,11 +535,12 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="104.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="6" width="67.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,14 +553,15 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -569,14 +574,15 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -589,12 +595,16 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="2">
+        <f>IF(F3="pozytywny",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -607,14 +617,18 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E32" si="0">IF(F4="pozytywny",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -627,14 +641,18 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -647,12 +665,16 @@
       <c r="D6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -665,12 +687,16 @@
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -683,12 +709,16 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -701,12 +731,16 @@
       <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -719,12 +753,16 @@
       <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -737,12 +775,16 @@
       <c r="D11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -755,14 +797,18 @@
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -775,14 +821,18 @@
       <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -795,12 +845,15 @@
       <c r="D14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -813,12 +866,15 @@
       <c r="D15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -831,14 +887,17 @@
       <c r="D16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -851,14 +910,17 @@
       <c r="D17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -871,12 +933,15 @@
       <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -889,12 +954,15 @@
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -907,12 +975,16 @@
       <c r="D20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -925,12 +997,16 @@
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -943,12 +1019,16 @@
       <c r="D22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -961,12 +1041,16 @@
       <c r="D23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -979,12 +1063,15 @@
       <c r="D24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="E24" s="2">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -997,12 +1084,15 @@
       <c r="D25" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -1015,12 +1105,15 @@
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1033,14 +1126,17 @@
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2">
+        <v>3</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -1053,14 +1149,17 @@
       <c r="D28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2">
+        <v>3</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -1073,14 +1172,17 @@
       <c r="D29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2">
+        <v>3</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -1093,12 +1195,16 @@
       <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -1111,12 +1217,16 @@
       <c r="D31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -1129,10 +1239,14 @@
       <c r="D32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="2"/>
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
skonczone punkty 2 3 4 z fb.
</commit_message>
<xml_diff>
--- a/dokumentacja/Karta testów - Dariusz Waltoś.xlsx
+++ b/dokumentacja/Karta testów - Dariusz Waltoś.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="32">
   <si>
     <t>Nazwisko</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Brak walidacji czy wprowadzona liczba jest stringiem</t>
+  </si>
+  <si>
+    <t>błędy</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -226,6 +229,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dane wyjściowe" xfId="1" builtinId="21"/>
@@ -236,6 +243,158 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2925571</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>106589</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="184731"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="pole tekstowe 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5080035" y="10353675"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4547124</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>58964</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="264560" cy="184731"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="pole tekstowe 13"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="6701588" y="10115550"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="pole tekstowe 14"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9744075" y="11934825"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -523,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,7 +733,9 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1248,9 +1409,34 @@
       </c>
       <c r="G32" s="2"/>
     </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>